<commit_message>
adaptation of test cases
</commit_message>
<xml_diff>
--- a/tests/assets/scripts5/data3-custom-voc-with-prefixes.xlsx
+++ b/tests/assets/scripts5/data3-custom-voc-with-prefixes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C88884C-8DA0-4A2A-ABAB-00A196171B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B90B35-C295-4202-93BD-CE8A3B4646FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatiefWerk" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
   <si>
     <t>CODE</t>
   </si>
@@ -297,12 +297,6 @@
     <t>prefix</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>foafAgent</t>
-  </si>
-  <si>
     <t>http://xmlns.com/foaf/0.1/</t>
   </si>
   <si>
@@ -334,6 +328,9 @@
   </si>
   <si>
     <t>ex</t>
+  </si>
+  <si>
+    <t>uri</t>
   </si>
 </sst>
 </file>
@@ -1096,10 +1093,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3F4CC-9B3F-47D0-9808-1EA0C7FA5DB2}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,16 +1129,16 @@
         <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1149,16 +1146,16 @@
         <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1169,10 +1166,10 @@
         <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1185,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46818EAE-7B8A-4FAC-8CCC-6F67FBA871BD}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,33 +1197,33 @@
         <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>